<commit_message>
update excel files and tables
</commit_message>
<xml_diff>
--- a/DataFiles_Excel/InternationalPieChart/HHSawardsNumberInternationalPieTable.xlsx
+++ b/DataFiles_Excel/InternationalPieChart/HHSawardsNumberInternationalPieTable.xlsx
@@ -1,44 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jim.ide\Desktop\annual-report-html2excel\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rickferris/Desktop/TaggsAR2016-master/DataFiles_Excel/InternationalPieChart/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="5340" yWindow="4660" windowWidth="28800" windowHeight="12800"/>
   </bookViews>
   <sheets>
     <sheet name="HHSawardsNumberInternationalPie" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>2016 Grant Dollars By Agency Table</t>
-  </si>
-  <si>
-    <t>This table displays the total number of grant awards each HHS agency awarded in FY 2016. It is provided as a text alternative to the interactive chart on the Awards page of this website.</t>
-  </si>
-  <si>
-    <t>HHS Total Number of Awards Description</t>
-  </si>
-  <si>
-    <t>Number of awards HHS awarded in FY 2016 by agency.</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>Total Number of Awards</t>
-  </si>
-  <si>
     <t>SAMHSA</t>
   </si>
   <si>
@@ -58,13 +48,31 @@
   </si>
   <si>
     <t>CDC</t>
+  </si>
+  <si>
+    <t>2016 International Grant Dollars By Agency Table</t>
+  </si>
+  <si>
+    <t>This table displays the total number of international grant awards each HHS agency awarded in FY 2016. It is provided as a text alternative to the interactive chart on the Awards page of this website.</t>
+  </si>
+  <si>
+    <t>HHS Total Number of International Awards Description</t>
+  </si>
+  <si>
+    <t>Number of international awards HHS awarded in FY 2016 by agency.</t>
+  </si>
+  <si>
+    <t>Agency</t>
+  </si>
+  <si>
+    <t>Total Number of International Awards</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +215,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -389,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -504,8 +528,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -548,15 +587,11 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -567,8 +602,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -597,11 +638,13 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -925,118 +968,121 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="6">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="2">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="2">
-        <v>541</v>
-      </c>
     </row>
   </sheetData>
+  <sortState ref="A10:B16">
+    <sortCondition ref="A10:A16"/>
+  </sortState>
   <mergeCells count="6">
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>

</xml_diff>